<commit_message>
My single function is back
</commit_message>
<xml_diff>
--- a/CH-081 Compaint grouping.xlsx
+++ b/CH-081 Compaint grouping.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6B9E697-A808-45C5-B35C-459618488EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F98F03-DCFE-40C1-B2FD-3454595CEEFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14810" yWindow="3350" windowWidth="14590" windowHeight="15410" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37440" yWindow="960" windowWidth="20380" windowHeight="15410" activeTab="1" xr2:uid="{0C7BD0E5-D882-4512-9DBE-2383CEE0CF63}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
     <sheet name="EDA" sheetId="2" r:id="rId2"/>
+    <sheet name="MySingleFunction" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">EDA!$B$2:$B$6</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">MySingleFunction!$B$2:$B$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Original!$B$2:$B$6</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -63,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="25">
   <si>
     <t>Date</t>
   </si>
@@ -1363,6 +1366,117 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>495298</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2168293-9EC8-4749-80AA-97EBCEDE30BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="723898" y="1647191"/>
+          <a:ext cx="3767457" cy="1028700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="2400" b="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Challenge</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AU" sz="2400" b="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t> 81</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-AU" sz="2400" b="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>:Total Distance! </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-AU" sz="1600" b="0">
+            <a:solidFill>
+              <a:sysClr val="windowText" lastClr="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1685,6 +1799,7 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2275,8 +2390,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A229CE8E-D357-4BCD-8903-EE8910956F27}">
   <dimension ref="B1:M75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3117,4 +3235,869 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E585767F-2EAB-4826-B79B-D0A0168961E7}">
+  <dimension ref="B1:M75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="3.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" customWidth="1"/>
+    <col min="9" max="9" width="9.6640625" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:13" s="4" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="38" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="H1" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="2:13" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="K2" s="33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="2:13" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="11">
+        <v>0</v>
+      </c>
+      <c r="D3" s="11">
+        <v>73</v>
+      </c>
+      <c r="E3" s="11">
+        <v>85</v>
+      </c>
+      <c r="F3" s="12">
+        <v>13</v>
+      </c>
+      <c r="H3" s="9">
+        <v>45388</v>
+      </c>
+      <c r="I3" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" s="25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="2:13" s="2" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="B4" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="11">
+        <v>73</v>
+      </c>
+      <c r="D4" s="11">
+        <v>0</v>
+      </c>
+      <c r="E4" s="11">
+        <v>91</v>
+      </c>
+      <c r="F4" s="12">
+        <v>41</v>
+      </c>
+      <c r="H4" s="9">
+        <v>45394</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="K4" s="25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="13">
+        <v>85</v>
+      </c>
+      <c r="D5" s="13">
+        <v>91</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0</v>
+      </c>
+      <c r="F5" s="14">
+        <v>31</v>
+      </c>
+      <c r="H5" s="34">
+        <v>45394</v>
+      </c>
+      <c r="I5" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" s="37">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="15">
+        <v>13</v>
+      </c>
+      <c r="D6" s="15">
+        <v>41</v>
+      </c>
+      <c r="E6" s="15">
+        <v>31</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0</v>
+      </c>
+      <c r="H6" s="9">
+        <v>45397</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="25">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="7" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="3"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="H7" s="9">
+        <v>45398</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="3"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="H8" s="10">
+        <v>45403</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="25">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="9" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="3"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="H9" s="26">
+        <v>45403</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="25">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="10" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="3"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="H10" s="26">
+        <v>45404</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="25">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="3"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="H11" s="26">
+        <v>45408</v>
+      </c>
+      <c r="I11" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="3"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="H12" s="26">
+        <v>45410</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="H13" s="26">
+        <v>45411</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="J13" s="23" t="s">
+        <v>19</v>
+      </c>
+      <c r="K13" s="28">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="H14" s="29">
+        <v>45412</v>
+      </c>
+      <c r="I14" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="K14" s="31">
+        <v>164</v>
+      </c>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="J15" s="5"/>
+      <c r="M15" s="1"/>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="J16" s="5"/>
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="J17" s="5"/>
+      <c r="M17" s="1"/>
+    </row>
+    <row r="18" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C18" s="17" t="str" cm="1">
+        <f t="array" ref="C18:F30">_xlfn.LET(
+_xlpm.l, _xlfn.TOCOL(B3:B6&amp;C2:F2),
+_xlpm.n, _xlfn.TOCOL(C3:F6),
+_xlpm.q,_xlfn.MAP(J3:J14,_xlfn.LAMBDA(_xlpm.x,_xlfn.LET(_xlpm.xc,SUBSTITUTE(_xlpm.x,",",""),_xlpm.z,_xlfn.REDUCE(0,_xlfn.SEQUENCE(LEN(_xlpm.xc)-1),_xlfn.LAMBDA(_xlpm.a,_xlpm.v,_xlfn.VSTACK(_xlpm.a,_xlfn.XLOOKUP(MID(_xlpm.xc,_xlpm.v,2),_xlpm.l,_xlpm.n)))),SUM(_xlpm.z)))),
+_xlfn.VSTACK(H2:K2,_xlfn.HSTACK(H3:J14,_xlpm.q))
+)</f>
+        <v>Date</v>
+      </c>
+      <c r="D18" s="18" t="str">
+        <v>Staff ID</v>
+      </c>
+      <c r="E18" s="8" t="str">
+        <v>Path</v>
+      </c>
+      <c r="F18" s="33" t="str">
+        <v>Distance</v>
+      </c>
+      <c r="J18" s="5"/>
+      <c r="M18" s="1"/>
+    </row>
+    <row r="19" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C19" s="9">
+        <v>45388</v>
+      </c>
+      <c r="D19" s="11" t="str">
+        <v>s-2</v>
+      </c>
+      <c r="E19" s="21" t="str">
+        <v>C,B</v>
+      </c>
+      <c r="F19" s="25">
+        <v>91</v>
+      </c>
+      <c r="H19" t="b" cm="1">
+        <f t="array" ref="H19:K31">H2:K14=_xlfn.ANCHORARRAY(C18)</f>
+        <v>1</v>
+      </c>
+      <c r="I19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J19" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" t="b">
+        <v>1</v>
+      </c>
+      <c r="M19" s="1"/>
+    </row>
+    <row r="20" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C20" s="9">
+        <v>45394</v>
+      </c>
+      <c r="D20" s="11" t="str">
+        <v>s-2</v>
+      </c>
+      <c r="E20" s="21" t="str">
+        <v>D,C</v>
+      </c>
+      <c r="F20" s="25">
+        <v>31</v>
+      </c>
+      <c r="H20" t="b">
+        <v>1</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" t="b">
+        <v>1</v>
+      </c>
+      <c r="M20" s="1"/>
+    </row>
+    <row r="21" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C21" s="34">
+        <v>45394</v>
+      </c>
+      <c r="D21" s="35" t="str">
+        <v>s-3</v>
+      </c>
+      <c r="E21" s="36" t="str">
+        <v>D,C,D</v>
+      </c>
+      <c r="F21" s="37">
+        <v>62</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="I21" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" t="b">
+        <v>1</v>
+      </c>
+      <c r="M21" s="1"/>
+    </row>
+    <row r="22" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C22" s="9">
+        <v>45397</v>
+      </c>
+      <c r="D22" s="11" t="str">
+        <v>s-3</v>
+      </c>
+      <c r="E22" s="22" t="str">
+        <v>A,C,B,A,B,A,C</v>
+      </c>
+      <c r="F22" s="25">
+        <v>480</v>
+      </c>
+      <c r="G22" s="19"/>
+      <c r="H22" t="b">
+        <v>1</v>
+      </c>
+      <c r="I22" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J22" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" t="b">
+        <v>1</v>
+      </c>
+      <c r="M22" s="1"/>
+    </row>
+    <row r="23" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C23" s="9">
+        <v>45398</v>
+      </c>
+      <c r="D23" s="13" t="str">
+        <v>s-1</v>
+      </c>
+      <c r="E23" s="22" t="str">
+        <v>A,B</v>
+      </c>
+      <c r="F23" s="25">
+        <v>73</v>
+      </c>
+      <c r="G23" s="19"/>
+      <c r="H23" t="b">
+        <v>1</v>
+      </c>
+      <c r="I23" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J23" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" t="b">
+        <v>1</v>
+      </c>
+      <c r="M23" s="1"/>
+    </row>
+    <row r="24" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C24" s="10">
+        <v>45403</v>
+      </c>
+      <c r="D24" s="13" t="str">
+        <v>s-1</v>
+      </c>
+      <c r="E24" s="22" t="str">
+        <v>A,C,B,A</v>
+      </c>
+      <c r="F24" s="25">
+        <v>249</v>
+      </c>
+      <c r="G24" s="19"/>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" t="b">
+        <v>1</v>
+      </c>
+      <c r="M24" s="1"/>
+    </row>
+    <row r="25" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C25" s="26">
+        <v>45403</v>
+      </c>
+      <c r="D25" s="27" t="str">
+        <v>s-3</v>
+      </c>
+      <c r="E25" s="22" t="str">
+        <v>A,B,C,A,B,A</v>
+      </c>
+      <c r="F25" s="25">
+        <v>395</v>
+      </c>
+      <c r="G25" s="19"/>
+      <c r="H25" t="b">
+        <v>1</v>
+      </c>
+      <c r="I25" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K25" t="b">
+        <v>1</v>
+      </c>
+      <c r="M25" s="1"/>
+    </row>
+    <row r="26" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C26" s="26">
+        <v>45404</v>
+      </c>
+      <c r="D26" s="27" t="str">
+        <v>s-2</v>
+      </c>
+      <c r="E26" s="22" t="str">
+        <v>A,B,C,D</v>
+      </c>
+      <c r="F26" s="25">
+        <v>195</v>
+      </c>
+      <c r="G26" s="19"/>
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" t="b">
+        <v>1</v>
+      </c>
+      <c r="M26" s="1"/>
+    </row>
+    <row r="27" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C27" s="26">
+        <v>45408</v>
+      </c>
+      <c r="D27" s="27" t="str">
+        <v>s-1</v>
+      </c>
+      <c r="E27" s="22" t="str">
+        <v>A,B</v>
+      </c>
+      <c r="F27" s="25">
+        <v>73</v>
+      </c>
+      <c r="G27" s="19"/>
+      <c r="H27" t="b">
+        <v>1</v>
+      </c>
+      <c r="I27" s="19" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" t="b">
+        <v>1</v>
+      </c>
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C28" s="26">
+        <v>45410</v>
+      </c>
+      <c r="D28" s="27" t="str">
+        <v>s-2</v>
+      </c>
+      <c r="E28" s="22" t="str">
+        <v>A,B</v>
+      </c>
+      <c r="F28" s="25">
+        <v>73</v>
+      </c>
+      <c r="G28" s="19"/>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K28" t="b">
+        <v>1</v>
+      </c>
+      <c r="M28" s="1"/>
+    </row>
+    <row r="29" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C29" s="26">
+        <v>45411</v>
+      </c>
+      <c r="D29" s="27" t="str">
+        <v>s-1</v>
+      </c>
+      <c r="E29" s="23" t="str">
+        <v>A,C</v>
+      </c>
+      <c r="F29" s="28">
+        <v>85</v>
+      </c>
+      <c r="G29" s="19"/>
+      <c r="H29" t="b">
+        <v>1</v>
+      </c>
+      <c r="I29" t="b">
+        <v>1</v>
+      </c>
+      <c r="J29" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" t="b">
+        <v>1</v>
+      </c>
+      <c r="M29" s="1"/>
+    </row>
+    <row r="30" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="C30" s="29">
+        <v>45412</v>
+      </c>
+      <c r="D30" s="30" t="str">
+        <v>s-1</v>
+      </c>
+      <c r="E30" s="24" t="str">
+        <v>A,B,C</v>
+      </c>
+      <c r="F30" s="31">
+        <v>164</v>
+      </c>
+      <c r="G30" s="19"/>
+      <c r="H30" t="b">
+        <v>1</v>
+      </c>
+      <c r="I30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" t="b">
+        <v>1</v>
+      </c>
+      <c r="M30" s="1"/>
+    </row>
+    <row r="31" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="D31" s="19"/>
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" t="b">
+        <v>1</v>
+      </c>
+      <c r="I31" t="b">
+        <v>1</v>
+      </c>
+      <c r="J31" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K31" t="b">
+        <v>1</v>
+      </c>
+      <c r="M31" s="1"/>
+    </row>
+    <row r="32" spans="3:13" x14ac:dyDescent="0.3">
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
+      <c r="F32" s="19"/>
+      <c r="G32" s="19"/>
+      <c r="J32" s="1"/>
+      <c r="M32" s="1"/>
+    </row>
+    <row r="33" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D33" s="19"/>
+      <c r="E33" s="19"/>
+      <c r="F33" s="19"/>
+      <c r="G33" s="19"/>
+      <c r="J33" s="1"/>
+      <c r="M33" s="1"/>
+    </row>
+    <row r="34" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="M34" s="1"/>
+    </row>
+    <row r="35" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="J35" s="19"/>
+      <c r="M35" s="1"/>
+    </row>
+    <row r="36" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="J36" s="19"/>
+      <c r="M36" s="1"/>
+    </row>
+    <row r="37" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="J37" s="19"/>
+      <c r="M37" s="1"/>
+    </row>
+    <row r="38" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="J38" s="19"/>
+      <c r="M38" s="1"/>
+    </row>
+    <row r="39" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="J39" s="19"/>
+      <c r="M39" s="1"/>
+    </row>
+    <row r="40" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="J40" s="19"/>
+      <c r="M40" s="1"/>
+    </row>
+    <row r="41" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="M41" s="1"/>
+    </row>
+    <row r="42" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="M42" s="1"/>
+    </row>
+    <row r="43" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="M43" s="1"/>
+    </row>
+    <row r="44" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="M44" s="1"/>
+    </row>
+    <row r="45" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="M45" s="1"/>
+    </row>
+    <row r="46" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="M46" s="1"/>
+    </row>
+    <row r="47" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="M47" s="1"/>
+    </row>
+    <row r="48" spans="4:13" x14ac:dyDescent="0.3">
+      <c r="M48" s="1"/>
+    </row>
+    <row r="49" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M49" s="1"/>
+    </row>
+    <row r="50" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M50" s="1"/>
+    </row>
+    <row r="51" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M51" s="1"/>
+    </row>
+    <row r="52" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M52" s="1"/>
+    </row>
+    <row r="53" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M53" s="1"/>
+    </row>
+    <row r="54" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M54" s="1"/>
+    </row>
+    <row r="55" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M55" s="1"/>
+    </row>
+    <row r="56" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M56" s="1"/>
+    </row>
+    <row r="57" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M57" s="1"/>
+    </row>
+    <row r="58" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M58" s="1"/>
+    </row>
+    <row r="59" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M59" s="1"/>
+    </row>
+    <row r="60" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M60" s="1"/>
+    </row>
+    <row r="61" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M61" s="1"/>
+    </row>
+    <row r="62" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M62" s="1"/>
+    </row>
+    <row r="63" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M63" s="1"/>
+    </row>
+    <row r="64" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M64" s="1"/>
+    </row>
+    <row r="65" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M65" s="1"/>
+    </row>
+    <row r="66" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M66" s="1"/>
+    </row>
+    <row r="67" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M67" s="1"/>
+    </row>
+    <row r="68" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M68" s="1"/>
+    </row>
+    <row r="69" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M69" s="1"/>
+    </row>
+    <row r="70" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M70" s="1"/>
+    </row>
+    <row r="71" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M71" s="1"/>
+    </row>
+    <row r="72" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M72" s="1"/>
+    </row>
+    <row r="73" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M73" s="1"/>
+    </row>
+    <row r="74" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M74" s="1"/>
+    </row>
+    <row r="75" spans="13:13" x14ac:dyDescent="0.3">
+      <c r="M75" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="H1:J1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>